<commit_message>
Changed format of led_layouts file.
</commit_message>
<xml_diff>
--- a/test/test_lpa_files/led-calibration/led_layouts.xlsx
+++ b/test/test_lpa_files/led-calibration/led_layouts.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19226"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455E5261-64C1-47E8-9176-F6AF926523DC}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,14 +15,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="51">
   <si>
     <t>LPA</t>
   </si>
   <si>
-    <t>Archive ID</t>
-  </si>
-  <si>
     <t>EO_01</t>
   </si>
   <si>
@@ -145,12 +143,6 @@
     <t>Channel</t>
   </si>
   <si>
-    <t>Top</t>
-  </si>
-  <si>
-    <t>Bot</t>
-  </si>
-  <si>
     <t>Layout</t>
   </si>
   <si>
@@ -173,12 +165,15 @@
   </si>
   <si>
     <t>Calibrated</t>
+  </si>
+  <si>
+    <t>LED Set</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -570,14 +565,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,33 +586,33 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
-        <v>45</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E2" s="6">
         <v>42398</v>
@@ -625,16 +620,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E3" s="6">
         <v>42398</v>
@@ -643,16 +638,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E4" s="6">
         <v>42398</v>
@@ -661,16 +656,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E5" s="6">
         <v>42398</v>
@@ -679,16 +674,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E6" s="6">
         <v>42398</v>
@@ -697,16 +692,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E7" s="6">
         <v>42398</v>
@@ -715,16 +710,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E8" s="6">
         <v>42398</v>
@@ -733,16 +728,16 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E9" s="6">
         <v>42398</v>
@@ -751,16 +746,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" t="s">
-        <v>44</v>
+        <v>33</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E10" s="5">
         <v>42399</v>
@@ -769,16 +764,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E11" s="5">
         <v>42439</v>
@@ -787,16 +782,16 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E12" s="5">
         <v>42399</v>
@@ -805,16 +800,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E13" s="5">
         <v>42439</v>
@@ -823,16 +818,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>44</v>
+        <v>35</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E14" s="5">
         <v>42399</v>
@@ -841,16 +836,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C15" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E15" s="5">
         <v>42439</v>
@@ -859,16 +854,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
+        <v>36</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E16" s="5">
         <v>42399</v>
@@ -877,16 +872,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E17" s="5">
         <v>42439</v>
@@ -895,16 +890,16 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" t="s">
-        <v>44</v>
+        <v>37</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E18" s="5">
         <v>42399</v>
@@ -913,16 +908,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E19" s="5">
         <v>42439</v>
@@ -931,16 +926,16 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E20" s="5">
         <v>42399</v>
@@ -949,16 +944,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E21" s="5">
         <v>42439</v>
@@ -967,16 +962,16 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" t="s">
-        <v>44</v>
+        <v>39</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E22" s="5">
         <v>42399</v>
@@ -985,16 +980,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E23" s="5">
         <v>42439</v>
@@ -1003,16 +998,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>41</v>
-      </c>
-      <c r="C24" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C24">
+        <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E24" s="5">
         <v>42399</v>
@@ -1021,16 +1016,16 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B25" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E25" s="5">
         <v>42439</v>
@@ -1039,16 +1034,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
         <v>44</v>
-      </c>
-      <c r="D26" t="s">
-        <v>47</v>
       </c>
       <c r="E26" s="5">
         <v>42403</v>
@@ -1057,16 +1052,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
         <v>44</v>
-      </c>
-      <c r="D27" t="s">
-        <v>47</v>
       </c>
       <c r="E27" s="5">
         <v>42403</v>
@@ -1075,16 +1070,16 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
         <v>44</v>
-      </c>
-      <c r="D28" t="s">
-        <v>47</v>
       </c>
       <c r="E28" s="5">
         <v>42403</v>
@@ -1093,16 +1088,16 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
         <v>44</v>
-      </c>
-      <c r="D29" t="s">
-        <v>47</v>
       </c>
       <c r="E29" s="5">
         <v>42403</v>
@@ -1111,16 +1106,16 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
         <v>44</v>
-      </c>
-      <c r="D30" t="s">
-        <v>47</v>
       </c>
       <c r="E30" s="5">
         <v>42403</v>
@@ -1129,16 +1124,16 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>43</v>
+        <v>37</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E31" s="5">
         <v>42439</v>
@@ -1147,16 +1142,16 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
-      </c>
-      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
         <v>44</v>
-      </c>
-      <c r="D32" t="s">
-        <v>47</v>
       </c>
       <c r="E32" s="5">
         <v>42403</v>
@@ -1165,16 +1160,16 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E33" s="5">
         <v>42439</v>
@@ -1183,16 +1178,16 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34" t="s">
         <v>44</v>
-      </c>
-      <c r="D34" t="s">
-        <v>47</v>
       </c>
       <c r="E34" s="5">
         <v>42403</v>
@@ -1201,16 +1196,16 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>41</v>
-      </c>
-      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
         <v>44</v>
-      </c>
-      <c r="D35" t="s">
-        <v>47</v>
       </c>
       <c r="E35" s="5">
         <v>42403</v>
@@ -1219,16 +1214,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
+      </c>
+      <c r="C36" s="4">
+        <v>2</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E36" s="5">
         <v>42426</v>
@@ -1237,64 +1232,64 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C37" t="s">
-        <v>44</v>
+        <v>34</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E37" s="3"/>
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" t="s">
-        <v>43</v>
+        <v>39</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E38" s="3"/>
       <c r="G38" s="3"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E39" s="3"/>
       <c r="G39" s="3"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" t="s">
-        <v>43</v>
+        <v>33</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E40" s="5">
         <v>42439</v>
@@ -1303,16 +1298,16 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" t="s">
-        <v>43</v>
+        <v>34</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E41" s="5">
         <v>42439</v>
@@ -1321,16 +1316,16 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E42" s="5">
         <v>42439</v>
@@ -1339,16 +1334,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B43" t="s">
-        <v>37</v>
-      </c>
-      <c r="C43" t="s">
-        <v>43</v>
+        <v>36</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E43" s="5">
         <v>42439</v>

</xml_diff>